<commit_message>
Updated DPM integration testfixture with hierarchy node labels
</commit_message>
<xml_diff>
--- a/yti-taxgen-test-commons/src/main/resources/test_fixtures/rds_source_config/dm_integration_fixture/ed-DOME-2018-1-members-and-hierarchies.xlsx
+++ b/yti-taxgen-test-commons/src/main/resources/test_fixtures/rds_source_config/dm_integration_fixture/ed-DOME-2018-1-members-and-hierarchies.xlsx
@@ -112,7 +112,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="29.700000000000003"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="31.900000000000002"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="18.15"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="26.4"/>
     <col min="4" max="4" bestFit="1" customWidth="1" width="23.099999999999998"/>
@@ -203,7 +203,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>d67ca944-01ab-4f4b-ba5f-0f2d6482c990</t>
+          <t>a68e6334-aedf-4a28-9964-057446f62d8c</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -268,7 +268,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="34.1"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="36.300000000000004"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="18.15"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="16.5"/>
     <col min="4" max="4" bestFit="1" customWidth="1" width="14.85"/>
@@ -335,7 +335,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>65316531-cc3e-437c-97b1-0be06c698afd</t>
+          <t>b8de6ed6-4461-433f-bd28-d117499ebf41</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -371,7 +371,7 @@
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>d87630e8-d994-454b-9c0f-3768da41a2d0</t>
+          <t>b8887fac-bca8-408f-8f84-6755e0e4370e</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
@@ -424,7 +424,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="31.900000000000002"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="28.6"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="18.15"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="14.85"/>
     <col min="4" max="4" bestFit="1" customWidth="1" width="24.75"/>
@@ -485,7 +485,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>5d0ddb13-ac77-407a-9e6b-c308bfef3146</t>
+          <t>4ffe9ff2-c8d2-4595-aa32-1155ac4598eb</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -524,7 +524,7 @@
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>f5d9f27f-2ec4-4444-adc0-687dc1f52da9</t>
+          <t>bc5cc9ce-7f49-4727-a2a6-ac7c390398b0</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
@@ -646,10 +646,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="27.500000000000004"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="36.300000000000004"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="11.549999999999999"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="14.85"/>
-    <col min="4" max="4" bestFit="1" customWidth="1" width="16.5"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" width="18.700000000000003"/>
     <col min="5" max="5" bestFit="1" customWidth="1" width="19.799999999999997"/>
     <col min="6" max="6" bestFit="1" customWidth="1" width="19.799999999999997"/>
     <col min="7" max="7" bestFit="1" customWidth="1" width="16.5"/>
@@ -695,7 +695,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>bbbab95b-e3cf-43fc-9cf5-aecb8105f1d9</t>
+          <t>29ce4f17-4468-436b-b4d8-300235d45e69</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -706,7 +706,7 @@
       <c r="C2" s="0"/>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>Member (fi, label)</t>
+          <t>Hierarchy node (fi, label)</t>
         </is>
       </c>
       <c r="E2" s="0"/>

</xml_diff>